<commit_message>
commit fin de journee bootstrap
</commit_message>
<xml_diff>
--- a/Bootstrap.xlsx
+++ b/Bootstrap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campuseni-my.sharepoint.com/personal/olivier_billant2022_campus-eni_fr/Documents/2022-02-07 - S3 - Html_et_CSS/TP/10 Bootstrap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{EA8F7B1C-3180-4A24-8BE8-41FECEDD268D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E3FDF58-AC6A-47F2-B03F-2F28FCED7310}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{EA8F7B1C-3180-4A24-8BE8-41FECEDD268D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4509B118-0721-4F5A-9DE3-33661A6CDBC4}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="15" windowWidth="16065" windowHeight="10710" xr2:uid="{1E058EA1-0163-41BC-93EF-FB270F0895AF}"/>
   </bookViews>
@@ -33,16 +33,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>Col 6</t>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Vide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +61,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,13 +84,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,17 +165,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,69 +491,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F77741-A075-4C4A-A495-26C463FD2AFB}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="B1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="7">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="C1" s="7">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="D1" s="7">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="E1" s="7">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="F1" s="7">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="G1" s="7">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="H1" s="7">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="I1" s="7">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="J1" s="7">
+      <c r="K1" s="1">
         <v>10</v>
       </c>
-      <c r="K1" s="7">
+      <c r="L1" s="1">
         <v>11</v>
       </c>
-      <c r="L1" s="7">
+      <c r="M1" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>